<commit_message>
APi works as well some template views but can t add any data yet
</commit_message>
<xml_diff>
--- a/CRUDCreateCode/data/input/models/Customer.xlsx
+++ b/CRUDCreateCode/data/input/models/Customer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tkax/dev/aimonetize/Backend/DjangoBasic/CRUDCreateCode/data/input/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49894079-18C3-2945-BB00-3282D1E92238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DA8620-AAB0-644E-851F-3645A345DB99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10100" yWindow="500" windowWidth="28000" windowHeight="21060" xr2:uid="{43DD2820-FE61-F645-B31F-194723807C3A}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <sheet name="forms" sheetId="6" r:id="rId6"/>
     <sheet name="html" sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="71">
   <si>
     <t>Variable</t>
   </si>
@@ -218,10 +218,47 @@
   </si>
   <si>
     <t xml:space="preserve">    class Meta:
-        ordering = ["name"]
-        fields = '__all__'
         verbose_name = 'Customer'
-        verbose_name_plural = "Customers"</t>
+        verbose_name_plural = 'Customers'</t>
+  </si>
+  <si>
+    <t>verbose_name</t>
+  </si>
+  <si>
+    <t>"Company Name"</t>
+  </si>
+  <si>
+    <t>"Active"</t>
+  </si>
+  <si>
+    <t>"AFM"</t>
+  </si>
+  <si>
+    <t>"First Name"</t>
+  </si>
+  <si>
+    <t>"Last Name"</t>
+  </si>
+  <si>
+    <t>"Email"</t>
+  </si>
+  <si>
+    <t>"Phone"</t>
+  </si>
+  <si>
+    <t>"Address"</t>
+  </si>
+  <si>
+    <t>"Created at"</t>
+  </si>
+  <si>
+    <t>"Updated at"</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>False</t>
   </si>
 </sst>
 </file>
@@ -268,12 +305,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,21 +626,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15A4BF7-DFDE-D24F-85FE-657339D228CC}">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:X11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="3" width="32.1640625" customWidth="1"/>
-    <col min="4" max="10" width="11.1640625" customWidth="1"/>
+    <col min="3" max="4" width="32.1640625" customWidth="1"/>
+    <col min="5" max="11" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -613,67 +651,70 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>42</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>43</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>38</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>39</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>44</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>55</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>49</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>53</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>27</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>46</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>47</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -683,23 +724,26 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="K2">
+      <c r="D2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2">
         <v>100</v>
       </c>
-      <c r="S2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T2" t="b">
-        <v>1</v>
-      </c>
-      <c r="U2" t="b">
-        <v>1</v>
-      </c>
-      <c r="W2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23">
+      <c r="T2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -709,20 +753,23 @@
       <c r="C3" t="s">
         <v>52</v>
       </c>
-      <c r="O3" t="b">
-        <v>0</v>
-      </c>
-      <c r="S3" t="b">
-        <v>1</v>
-      </c>
-      <c r="U3" t="b">
-        <v>1</v>
-      </c>
-      <c r="W3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23">
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -732,26 +779,26 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="K4">
-        <v>9</v>
-      </c>
-      <c r="M4" t="b">
-        <v>1</v>
-      </c>
-      <c r="N4" t="b">
-        <v>1</v>
-      </c>
-      <c r="S4" t="b">
-        <v>1</v>
-      </c>
-      <c r="U4" t="b">
-        <v>1</v>
-      </c>
-      <c r="W4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23">
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -761,20 +808,23 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="K5">
+      <c r="D5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L5">
         <v>100</v>
       </c>
-      <c r="S5" t="b">
-        <v>1</v>
-      </c>
-      <c r="U5" t="b">
-        <v>1</v>
-      </c>
-      <c r="W5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23">
+      <c r="T5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -784,20 +834,23 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="K6">
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
+      <c r="L6">
         <v>100</v>
       </c>
-      <c r="S6" t="b">
-        <v>1</v>
-      </c>
-      <c r="U6" t="b">
-        <v>1</v>
-      </c>
-      <c r="W6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23">
+      <c r="T6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -807,20 +860,23 @@
       <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="L7" t="b">
-        <v>1</v>
-      </c>
-      <c r="S7" t="b">
-        <v>1</v>
-      </c>
-      <c r="U7" t="b">
-        <v>1</v>
-      </c>
-      <c r="W7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23">
+      <c r="D7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -830,26 +886,29 @@
       <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="K8">
+      <c r="D8" t="s">
+        <v>65</v>
+      </c>
+      <c r="L8">
         <v>15</v>
       </c>
-      <c r="M8" t="b">
-        <v>1</v>
-      </c>
-      <c r="N8" t="b">
-        <v>1</v>
-      </c>
-      <c r="S8" t="b">
-        <v>1</v>
-      </c>
-      <c r="U8" t="b">
-        <v>1</v>
-      </c>
-      <c r="W8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23">
+      <c r="N8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -859,23 +918,26 @@
       <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="M9" t="b">
-        <v>1</v>
-      </c>
-      <c r="N9" t="b">
-        <v>1</v>
-      </c>
-      <c r="S9" t="b">
-        <v>1</v>
-      </c>
-      <c r="U9" t="b">
-        <v>1</v>
-      </c>
-      <c r="W9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23">
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -885,20 +947,21 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="P10" t="b">
-        <v>1</v>
-      </c>
-      <c r="S10" t="b">
-        <v>1</v>
-      </c>
-      <c r="U10" t="b">
-        <v>1</v>
-      </c>
-      <c r="W10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23">
+      <c r="D10" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="X10" s="3"/>
+    </row>
+    <row r="11" spans="1:24">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -908,18 +971,19 @@
       <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="Q11" t="b">
-        <v>1</v>
-      </c>
-      <c r="S11" t="b">
-        <v>1</v>
-      </c>
-      <c r="U11" t="b">
-        <v>1</v>
-      </c>
-      <c r="W11" t="b">
-        <v>1</v>
-      </c>
+      <c r="D11" t="s">
+        <v>68</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="X11" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -932,7 +996,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -956,7 +1020,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="85">
+    <row r="3" spans="1:2" ht="51">
       <c r="A3" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
createde the dbgraph file and cleaned the model xslx files
</commit_message>
<xml_diff>
--- a/CRUDCreateCode/data/input/models/Customer.xlsx
+++ b/CRUDCreateCode/data/input/models/Customer.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tkax/dev/aimonetize/Backend/DjangoBasic/CRUDCreateCode/data/input/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DA8620-AAB0-644E-851F-3645A345DB99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00910505-6748-584E-99F7-BE7F231987CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10100" yWindow="500" windowWidth="28000" windowHeight="21060" xr2:uid="{43DD2820-FE61-F645-B31F-194723807C3A}"/>
+    <workbookView xWindow="2240" yWindow="760" windowWidth="28000" windowHeight="18880" activeTab="1" xr2:uid="{43DD2820-FE61-F645-B31F-194723807C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
-    <sheet name="model_functions" sheetId="7" r:id="rId2"/>
-    <sheet name="serializers" sheetId="2" r:id="rId3"/>
-    <sheet name="views" sheetId="3" r:id="rId4"/>
-    <sheet name="urls" sheetId="4" r:id="rId5"/>
-    <sheet name="forms" sheetId="6" r:id="rId6"/>
-    <sheet name="html" sheetId="5" r:id="rId7"/>
+    <sheet name="admin" sheetId="9" r:id="rId2"/>
+    <sheet name="apps" sheetId="10" r:id="rId3"/>
+    <sheet name="model_functions" sheetId="7" r:id="rId4"/>
+    <sheet name="serializers" sheetId="2" r:id="rId5"/>
+    <sheet name="views" sheetId="3" r:id="rId6"/>
+    <sheet name="urls" sheetId="4" r:id="rId7"/>
+    <sheet name="forms" sheetId="6" r:id="rId8"/>
+    <sheet name="html" sheetId="5" r:id="rId9"/>
+    <sheet name="signals" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="76">
   <si>
     <t>Variable</t>
   </si>
@@ -150,10 +153,6 @@
   </si>
   <si>
     <t>functions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">def __str__(): 
-    </t>
   </si>
   <si>
     <t>ID</t>
@@ -259,13 +258,31 @@
   </si>
   <si>
     <t>False</t>
+  </si>
+  <si>
+    <t>model_name</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>history</t>
+  </si>
+  <si>
+    <t>HistoricalRecords</t>
+  </si>
+  <si>
+    <t>HistoricalRecords()</t>
+  </si>
+  <si>
+    <t>"History"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -283,6 +300,13 @@
       <sz val="10"/>
       <color rgb="FF0C0D0E"/>
       <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -305,13 +329,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,9 +355,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -370,7 +395,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -476,7 +501,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -618,7 +643,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -626,21 +651,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15A4BF7-DFDE-D24F-85FE-657339D228CC}">
-  <dimension ref="A1:X11"/>
+  <dimension ref="A1:Y12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="4" width="32.1640625" customWidth="1"/>
-    <col min="5" max="11" width="11.1640625" customWidth="1"/>
+    <col min="2" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="5" width="32.1640625" customWidth="1"/>
+    <col min="6" max="12" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -648,73 +673,76 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>58</v>
-      </c>
       <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" t="s">
-        <v>40</v>
-      </c>
       <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" t="s">
         <v>45</v>
       </c>
-      <c r="H1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>54</v>
-      </c>
-      <c r="R1" t="s">
-        <v>55</v>
-      </c>
-      <c r="S1" t="s">
-        <v>49</v>
-      </c>
-      <c r="T1" t="s">
-        <v>53</v>
-      </c>
-      <c r="U1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>46</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>47</v>
       </c>
-      <c r="X1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24">
+    </row>
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -722,54 +750,60 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2">
+        <v>100</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
         <v>59</v>
       </c>
-      <c r="L2">
-        <v>100</v>
-      </c>
-      <c r="T2" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="U2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" t="s">
-        <v>60</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="U3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -777,28 +811,31 @@
         <v>26</v>
       </c>
       <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
-        <v>61</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>69</v>
+      <c r="E4" t="s">
+        <v>60</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24">
+        <v>68</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -806,25 +843,28 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
-        <v>62</v>
-      </c>
-      <c r="L5">
+      <c r="E5" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5">
         <v>100</v>
       </c>
-      <c r="T5" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="V5" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="X5" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24">
+      <c r="U5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -832,25 +872,28 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
-        <v>63</v>
-      </c>
-      <c r="L6">
+      <c r="E6" t="s">
+        <v>62</v>
+      </c>
+      <c r="M6">
         <v>100</v>
       </c>
-      <c r="T6" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="V6" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="X6" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24">
+      <c r="U6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -858,25 +901,28 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
-        <v>64</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="T7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="V7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="X7" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24">
+      <c r="E7" t="s">
+        <v>63</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -884,31 +930,34 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
-        <v>65</v>
-      </c>
-      <c r="L8">
+      <c r="E8" t="s">
+        <v>64</v>
+      </c>
+      <c r="M8">
         <v>15</v>
       </c>
-      <c r="N8" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="O8" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="V8" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="X8" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24">
+        <v>68</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -916,28 +965,31 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="D9" t="s">
-        <v>66</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>69</v>
+      <c r="E9" t="s">
+        <v>65</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="T9" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="V9" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="X9" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24">
+        <v>68</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -945,23 +997,26 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="T10" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="V10" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="X10" s="3"/>
-    </row>
-    <row r="11" spans="1:24">
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y10" s="3"/>
+    </row>
+    <row r="11" spans="1:25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -969,21 +1024,41 @@
         <v>22</v>
       </c>
       <c r="C11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" t="s">
         <v>24</v>
       </c>
-      <c r="D11" t="s">
-        <v>68</v>
-      </c>
-      <c r="R11" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="T11" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="V11" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="X11" s="3"/>
+      <c r="E11" t="s">
+        <v>67</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y11" s="3"/>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" t="s">
+        <v>75</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -991,12 +1066,81 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB03DE8D-4BA4-BC4F-A158-DEBB72F32FA9}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3DDAA4-8DA6-D34B-8453-E75F7C707A37}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408682E9-ACFC-2244-925F-5FCEC9275D28}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0437A48-3006-3A4F-8E27-223B720E6D4E}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1006,7 +1150,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
         <v>35</v>
@@ -1017,15 +1161,15 @@
         <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="51">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1036,12 +1180,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5DCB6D-D252-554A-AA6D-EF7613AF9735}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1051,56 +1195,14 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="34">
-      <c r="A2" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCCD04C-73D9-ED48-83F8-2B0724B93DB6}">
-  <dimension ref="D1"/>
-  <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData>
-    <row r="1" spans="4:4">
-      <c r="D1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9DE9946-B381-0247-B0AA-E67A7DD58800}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>35</v>
-      </c>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1108,17 +1210,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D736743-F982-B748-AF4D-941EEF6BA5FF}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCCD04C-73D9-ED48-83F8-2B0724B93DB6}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1128,6 +1233,52 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9DE9946-B381-0247-B0AA-E67A7DD58800}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D736743-F982-B748-AF4D-941EEF6BA5FF}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80EF3DF2-641B-5E44-AA75-D6FFD80FBD8B}">
   <dimension ref="A1:B5"/>
   <sheetViews>

</xml_diff>